<commit_message>
Updates to Age files from last week of Aug-first week of Sept
	new file:   agebycoverhists.py
	modified:   agefunctions_draft1.py
		Updated with script to create the condition-age layer
	modified:   agelookuptable.csv
		Updated after review of all descriptions and inclusive of nonseral age
	modified:   maxagecount.xlsx
		Updated after review of all descriptions and fixing of nonseral age
</commit_message>
<xml_diff>
--- a/maxagecount.xlsx
+++ b/maxagecount.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21980" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21760" windowHeight="18200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MaxAgeCount 0905" sheetId="2" r:id="rId2"/>
+    <sheet name="Old MaxAgeCount" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="54">
   <si>
     <t>cov,</t>
   </si>
@@ -64,16 +66,149 @@
   </si>
   <si>
     <t>40,41,42,43 = aspen specific</t>
+  </si>
+  <si>
+    <t>Cover</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Pixel Count</t>
+  </si>
+  <si>
+    <t>28000 acres</t>
+  </si>
+  <si>
+    <t>20600 acres</t>
+  </si>
+  <si>
+    <t>91400 acres</t>
+  </si>
+  <si>
+    <t>17200 acres</t>
+  </si>
+  <si>
+    <t>(3</t>
+  </si>
+  <si>
+    <t>(4</t>
+  </si>
+  <si>
+    <t>(5</t>
+  </si>
+  <si>
+    <t>(7</t>
+  </si>
+  <si>
+    <t>(8</t>
+  </si>
+  <si>
+    <t>(9</t>
+  </si>
+  <si>
+    <t>(11</t>
+  </si>
+  <si>
+    <t>(12</t>
+  </si>
+  <si>
+    <t>(13</t>
+  </si>
+  <si>
+    <t>(14</t>
+  </si>
+  <si>
+    <t>(15</t>
+  </si>
+  <si>
+    <t>(16</t>
+  </si>
+  <si>
+    <t>(18</t>
+  </si>
+  <si>
+    <t>(20</t>
+  </si>
+  <si>
+    <t>(19</t>
+  </si>
+  <si>
+    <t>(17</t>
+  </si>
+  <si>
+    <t>(21</t>
+  </si>
+  <si>
+    <t>(22</t>
+  </si>
+  <si>
+    <t>(23</t>
+  </si>
+  <si>
+    <t>(25</t>
+  </si>
+  <si>
+    <t>(27</t>
+  </si>
+  <si>
+    <t>(26</t>
+  </si>
+  <si>
+    <t>(24</t>
+  </si>
+  <si>
+    <t>(30</t>
+  </si>
+  <si>
+    <t>(31</t>
+  </si>
+  <si>
+    <t>(32</t>
+  </si>
+  <si>
+    <t>(1</t>
+  </si>
+  <si>
+    <t>(2</t>
+  </si>
+  <si>
+    <t>(6</t>
+  </si>
+  <si>
+    <t>(10</t>
+  </si>
+  <si>
+    <t>(28</t>
+  </si>
+  <si>
+    <t>(29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,14 +237,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1727,6 +1894,2702 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>13805</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>77293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>1095</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>1901</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>259</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>130367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>23921</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>31</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>13021</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>21</v>
+      </c>
+      <c r="C41">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>18</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>6567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>51090</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>18</v>
+      </c>
+      <c r="B49" s="1">
+        <v>22</v>
+      </c>
+      <c r="C49">
+        <v>41644</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>18</v>
+      </c>
+      <c r="B50">
+        <v>31</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>18</v>
+      </c>
+      <c r="B51">
+        <v>32</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>20</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>20</v>
+      </c>
+      <c r="B53">
+        <v>21</v>
+      </c>
+      <c r="C53">
+        <v>9557</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>20</v>
+      </c>
+      <c r="B54">
+        <v>22</v>
+      </c>
+      <c r="C54">
+        <v>6025</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>31</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>20</v>
+      </c>
+      <c r="B56">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>19</v>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+      <c r="C57">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>19</v>
+      </c>
+      <c r="B58">
+        <v>21</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>19</v>
+      </c>
+      <c r="B59">
+        <v>22</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>19</v>
+      </c>
+      <c r="B60">
+        <v>31</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>19</v>
+      </c>
+      <c r="B61">
+        <v>32</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>17</v>
+      </c>
+      <c r="B62">
+        <v>40</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>41</v>
+      </c>
+      <c r="C63">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>17</v>
+      </c>
+      <c r="B64">
+        <v>42</v>
+      </c>
+      <c r="C64">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>17</v>
+      </c>
+      <c r="B65">
+        <v>31</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>17</v>
+      </c>
+      <c r="B66">
+        <v>43</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>21</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>6586</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>21</v>
+      </c>
+      <c r="B68">
+        <v>21</v>
+      </c>
+      <c r="C68">
+        <v>6915</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>21</v>
+      </c>
+      <c r="B69">
+        <v>22</v>
+      </c>
+      <c r="C69">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>21</v>
+      </c>
+      <c r="B70">
+        <v>32</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>31</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>22</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>22</v>
+      </c>
+      <c r="B73">
+        <v>21</v>
+      </c>
+      <c r="C73">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>22</v>
+      </c>
+      <c r="B74">
+        <v>22</v>
+      </c>
+      <c r="C74">
+        <v>11945</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>22</v>
+      </c>
+      <c r="B75">
+        <v>31</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>22</v>
+      </c>
+      <c r="B76">
+        <v>32</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>23</v>
+      </c>
+      <c r="B77">
+        <v>40</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>23</v>
+      </c>
+      <c r="B78">
+        <v>41</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>23</v>
+      </c>
+      <c r="B79">
+        <v>43</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>25</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>27600</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>25</v>
+      </c>
+      <c r="B81" s="1">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>190917</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>25</v>
+      </c>
+      <c r="B82" s="1">
+        <v>22</v>
+      </c>
+      <c r="C82">
+        <v>220191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>25</v>
+      </c>
+      <c r="B83">
+        <v>31</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>25</v>
+      </c>
+      <c r="B84">
+        <v>32</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>27</v>
+      </c>
+      <c r="B85">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>19907</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>27</v>
+      </c>
+      <c r="B86">
+        <v>21</v>
+      </c>
+      <c r="C86">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>27</v>
+      </c>
+      <c r="B87">
+        <v>22</v>
+      </c>
+      <c r="C87">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>27</v>
+      </c>
+      <c r="B88">
+        <v>31</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>27</v>
+      </c>
+      <c r="B89">
+        <v>32</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>26</v>
+      </c>
+      <c r="B90">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>26</v>
+      </c>
+      <c r="B91">
+        <v>21</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>26</v>
+      </c>
+      <c r="B92">
+        <v>22</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>26</v>
+      </c>
+      <c r="B93">
+        <v>31</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>26</v>
+      </c>
+      <c r="B94">
+        <v>32</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>24</v>
+      </c>
+      <c r="B95">
+        <v>40</v>
+      </c>
+      <c r="C95">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>24</v>
+      </c>
+      <c r="B96">
+        <v>41</v>
+      </c>
+      <c r="C96">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>24</v>
+      </c>
+      <c r="B97">
+        <v>42</v>
+      </c>
+      <c r="C97">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>24</v>
+      </c>
+      <c r="B98">
+        <v>31</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>24</v>
+      </c>
+      <c r="B99">
+        <v>43</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100">
+        <v>30</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>30</v>
+      </c>
+      <c r="B101">
+        <v>21</v>
+      </c>
+      <c r="C101">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>30</v>
+      </c>
+      <c r="B102">
+        <v>22</v>
+      </c>
+      <c r="C102">
+        <v>4213</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>30</v>
+      </c>
+      <c r="B103">
+        <v>31</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>30</v>
+      </c>
+      <c r="B104">
+        <v>32</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>31</v>
+      </c>
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>31</v>
+      </c>
+      <c r="B106">
+        <v>21</v>
+      </c>
+      <c r="C106">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>31</v>
+      </c>
+      <c r="B107">
+        <v>22</v>
+      </c>
+      <c r="C107">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>31</v>
+      </c>
+      <c r="B108">
+        <v>31</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>31</v>
+      </c>
+      <c r="B109">
+        <v>32</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
+        <v>32</v>
+      </c>
+      <c r="B110">
+        <v>40</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>32</v>
+      </c>
+      <c r="B111">
+        <v>41</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112">
+        <v>32</v>
+      </c>
+      <c r="B112">
+        <v>43</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>60584</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>98556</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115">
+        <v>6</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>35252</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116">
+        <v>10</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>38262</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>28</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>26178</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118">
+        <v>29</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>93411</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C117"/>
+  <sheetViews>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>13805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>77293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>42</v>
+      </c>
+      <c r="C18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>130367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>23921</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37">
+        <v>31</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>13021</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>22</v>
+      </c>
+      <c r="C39">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43">
+        <v>22</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>6567</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47">
+        <v>21</v>
+      </c>
+      <c r="C47">
+        <v>51090</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48">
+        <v>22</v>
+      </c>
+      <c r="C48">
+        <v>41644</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49">
+        <v>31</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50">
+        <v>32</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52">
+        <v>21</v>
+      </c>
+      <c r="C52">
+        <v>9557</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
+      <c r="C53">
+        <v>6025</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54">
+        <v>31</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55">
+        <v>32</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58">
+        <v>22</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59">
+        <v>31</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60">
+        <v>32</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61">
+        <v>40</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62">
+        <v>41</v>
+      </c>
+      <c r="C62">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63">
+        <v>42</v>
+      </c>
+      <c r="C63">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64">
+        <v>31</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65">
+        <v>43</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66">
+        <v>10</v>
+      </c>
+      <c r="C66">
+        <v>6586</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67">
+        <v>21</v>
+      </c>
+      <c r="C67">
+        <v>6915</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68">
+        <v>22</v>
+      </c>
+      <c r="C68">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69">
+        <v>32</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70">
+        <v>31</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72">
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73">
+        <v>22</v>
+      </c>
+      <c r="C73">
+        <v>11945</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74">
+        <v>31</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75">
+        <v>32</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76">
+        <v>40</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77">
+        <v>41</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>40</v>
+      </c>
+      <c r="B78">
+        <v>43</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>27600</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>190917</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81">
+        <v>22</v>
+      </c>
+      <c r="C81">
+        <v>220191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82">
+        <v>31</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>41</v>
+      </c>
+      <c r="B83">
+        <v>32</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>19907</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85">
+        <v>21</v>
+      </c>
+      <c r="C85">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86">
+        <v>22</v>
+      </c>
+      <c r="C86">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87">
+        <v>31</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88">
+        <v>32</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>43</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>43</v>
+      </c>
+      <c r="B90">
+        <v>21</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>43</v>
+      </c>
+      <c r="B91">
+        <v>22</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>43</v>
+      </c>
+      <c r="B92">
+        <v>31</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93">
+        <v>32</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>44</v>
+      </c>
+      <c r="B94">
+        <v>40</v>
+      </c>
+      <c r="C94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>44</v>
+      </c>
+      <c r="B95">
+        <v>41</v>
+      </c>
+      <c r="C95">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>44</v>
+      </c>
+      <c r="B96">
+        <v>42</v>
+      </c>
+      <c r="C96">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>44</v>
+      </c>
+      <c r="B97">
+        <v>31</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>44</v>
+      </c>
+      <c r="B98">
+        <v>43</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>45</v>
+      </c>
+      <c r="B99">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>45</v>
+      </c>
+      <c r="B100">
+        <v>21</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101">
+        <v>22</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>45</v>
+      </c>
+      <c r="B102">
+        <v>31</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103">
+        <v>32</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>46</v>
+      </c>
+      <c r="B104">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105">
+        <v>21</v>
+      </c>
+      <c r="C105">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106">
+        <v>22</v>
+      </c>
+      <c r="C106">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>46</v>
+      </c>
+      <c r="B107">
+        <v>31</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>46</v>
+      </c>
+      <c r="B108">
+        <v>32</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>47</v>
+      </c>
+      <c r="B109">
+        <v>40</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>47</v>
+      </c>
+      <c r="B110">
+        <v>41</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>47</v>
+      </c>
+      <c r="B111">
+        <v>43</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>48</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>49</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>50</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>51</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>53</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>